<commit_message>
Shilpa- master DSLgo first commit
</commit_message>
<xml_diff>
--- a/excel/LoginDetails.xlsx
+++ b/excel/LoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shilp\eclipse-workspace\DslgoSnam\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717CE1A8-E792-4A42-A826-3E7B84304A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFEC94A-49CF-459B-93CB-B93FBB54CBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="430" yWindow="1090" windowWidth="8520" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Username</t>
   </si>
@@ -36,29 +36,34 @@
     <t>Ninjastars</t>
   </si>
   <si>
+    <t>Expected message</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>jfvnjdf</t>
+  </si>
+  <si>
     <t>stars@2023</t>
-  </si>
-  <si>
-    <t>Expected message</t>
-  </si>
-  <si>
-    <t>Invalid password</t>
-  </si>
-  <si>
-    <t>Login successful</t>
-  </si>
-  <si>
-    <t>jfvnjdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,10 +92,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -105,8 +111,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,7 +398,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -406,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -414,21 +424,18 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>